<commit_message>
Update with Philadelphia County data
</commit_message>
<xml_diff>
--- a/data/philadelphia_combination.xlsx
+++ b/data/philadelphia_combination.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10808"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mreitsma/COVID/vaccination_analysis/KFF Analysis/vaccination_coverage_by_race/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mreitsma/COVID/vaccination_analysis/KFF Analysis/dashboard/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87E9D923-5F1D-CC4E-9B96-31A00B4F6ABB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C2D2FE1-20DC-484B-B318-AAB2EBE2DDFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-14920" yWindow="-19060" windowWidth="27240" windowHeight="15940" xr2:uid="{622412A1-A2BA-6948-8976-B67926182B35}"/>
+    <workbookView xWindow="14600" yWindow="-21100" windowWidth="38400" windowHeight="21100" xr2:uid="{622412A1-A2BA-6948-8976-B67926182B35}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="399" uniqueCount="30">
   <si>
     <t>White</t>
   </si>
@@ -170,7 +170,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -182,6 +182,10 @@
     <xf numFmtId="4" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="4" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -496,10 +500,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93808F88-E545-C84E-A629-6B896EB63490}">
-  <dimension ref="A1:S111"/>
+  <dimension ref="A1:S191"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A90" workbookViewId="0">
-      <selection activeCell="I105" sqref="I105:J105"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A147" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K184" sqref="K184"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4370,7 +4375,7 @@
         <v>6057.5971961977684</v>
       </c>
     </row>
-    <row r="101" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:19" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A101" s="1">
         <v>44284</v>
       </c>
@@ -4792,6 +4797,3086 @@
       <c r="J111">
         <f t="shared" si="127"/>
         <v>-2.9725924885042062E-5</v>
+      </c>
+    </row>
+    <row r="112" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A112" s="1">
+        <v>44256</v>
+      </c>
+      <c r="B112" t="s">
+        <v>18</v>
+      </c>
+      <c r="C112" t="s">
+        <v>26</v>
+      </c>
+      <c r="D112">
+        <v>0.2</v>
+      </c>
+      <c r="E112">
+        <v>0.13</v>
+      </c>
+      <c r="F112">
+        <v>0.09</v>
+      </c>
+      <c r="G112">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="H112">
+        <v>0.1</v>
+      </c>
+      <c r="O112">
+        <v>469225.79599999997</v>
+      </c>
+      <c r="P112">
+        <v>511877.33199999999</v>
+      </c>
+      <c r="Q112">
+        <v>183840</v>
+      </c>
+      <c r="R112">
+        <v>99881.19</v>
+      </c>
+      <c r="S112">
+        <v>31570.628000000001</v>
+      </c>
+    </row>
+    <row r="113" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A113" s="1">
+        <v>44256</v>
+      </c>
+      <c r="B113" t="s">
+        <v>18</v>
+      </c>
+      <c r="C113" t="s">
+        <v>19</v>
+      </c>
+      <c r="D113">
+        <f>D112*O112</f>
+        <v>93845.159199999995</v>
+      </c>
+      <c r="E113">
+        <f>E112*P112</f>
+        <v>66544.053159999996</v>
+      </c>
+      <c r="F113">
+        <f>F112*Q112</f>
+        <v>16545.599999999999</v>
+      </c>
+      <c r="G113">
+        <f>G112*R112</f>
+        <v>13983.366600000001</v>
+      </c>
+      <c r="H113">
+        <f>H112*S112</f>
+        <v>3157.0628000000002</v>
+      </c>
+      <c r="K113">
+        <v>309203</v>
+      </c>
+      <c r="L113">
+        <f>K113-(SUM(D113:H113))</f>
+        <v>115127.75823999997</v>
+      </c>
+      <c r="O113">
+        <v>469225.79599999997</v>
+      </c>
+      <c r="P113">
+        <v>511877.33199999999</v>
+      </c>
+      <c r="Q113">
+        <v>183840</v>
+      </c>
+      <c r="R113">
+        <v>99881.19</v>
+      </c>
+      <c r="S113">
+        <v>31570.628000000001</v>
+      </c>
+    </row>
+    <row r="114" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A114" s="1">
+        <v>44256</v>
+      </c>
+      <c r="B114" t="s">
+        <v>18</v>
+      </c>
+      <c r="C114" t="s">
+        <v>20</v>
+      </c>
+      <c r="D114">
+        <f>D113+(D113/(SUM($D113:$H113)))*$L113</f>
+        <v>149515.23180891486</v>
+      </c>
+      <c r="E114">
+        <f t="shared" ref="E114:H114" si="128">E113+(E113/(SUM($D113:$H113)))*$L113</f>
+        <v>106018.78262594661</v>
+      </c>
+      <c r="F114">
+        <f t="shared" si="128"/>
+        <v>26360.648119797548</v>
+      </c>
+      <c r="G114">
+        <f t="shared" si="128"/>
+        <v>22278.467173915116</v>
+      </c>
+      <c r="H114">
+        <f t="shared" si="128"/>
+        <v>5029.8702714258043</v>
+      </c>
+    </row>
+    <row r="115" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A115" s="1">
+        <v>44256</v>
+      </c>
+      <c r="B115" t="s">
+        <v>21</v>
+      </c>
+      <c r="C115" t="s">
+        <v>28</v>
+      </c>
+      <c r="D115" s="6">
+        <v>0.89</v>
+      </c>
+      <c r="E115" s="6">
+        <v>0.03</v>
+      </c>
+      <c r="F115" s="6">
+        <v>0.02</v>
+      </c>
+      <c r="G115" s="5">
+        <v>2.1089911618145641E-3</v>
+      </c>
+      <c r="H115" s="6">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="I115" s="5">
+        <v>2.156462782801142E-4</v>
+      </c>
+      <c r="J115" s="4">
+        <v>1.7674898883607312E-3</v>
+      </c>
+    </row>
+    <row r="116" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A116" s="1">
+        <v>44256</v>
+      </c>
+      <c r="B116" t="s">
+        <v>21</v>
+      </c>
+      <c r="C116" t="s">
+        <v>19</v>
+      </c>
+      <c r="D116">
+        <f>D115*$K116</f>
+        <v>1645158.77</v>
+      </c>
+      <c r="E116">
+        <f t="shared" ref="E116:J116" si="129">E115*$K116</f>
+        <v>55454.79</v>
+      </c>
+      <c r="F116">
+        <f t="shared" si="129"/>
+        <v>36969.86</v>
+      </c>
+      <c r="G116">
+        <f t="shared" si="129"/>
+        <v>3898.4553996760892</v>
+      </c>
+      <c r="H116">
+        <f t="shared" si="129"/>
+        <v>129394.51000000001</v>
+      </c>
+      <c r="I116">
+        <f t="shared" si="129"/>
+        <v>398.62063587684315</v>
+      </c>
+      <c r="J116">
+        <f t="shared" si="129"/>
+        <v>3267.192686205593</v>
+      </c>
+      <c r="K116" s="2">
+        <v>1848493</v>
+      </c>
+    </row>
+    <row r="117" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A117" s="1">
+        <v>44256</v>
+      </c>
+      <c r="B117" t="s">
+        <v>21</v>
+      </c>
+      <c r="C117" t="s">
+        <v>29</v>
+      </c>
+      <c r="D117">
+        <v>0.77694459599999999</v>
+      </c>
+      <c r="E117">
+        <v>0.10407799600000001</v>
+      </c>
+      <c r="G117">
+        <v>4.0013660000000001E-3</v>
+      </c>
+      <c r="H117">
+        <v>0.10407799600000001</v>
+      </c>
+      <c r="I117">
+        <v>1.4221746E-2</v>
+      </c>
+      <c r="J117">
+        <v>1.737557E-3</v>
+      </c>
+      <c r="K117" s="2"/>
+    </row>
+    <row r="118" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A118" s="1">
+        <v>44256</v>
+      </c>
+      <c r="B118" t="s">
+        <v>21</v>
+      </c>
+      <c r="C118" t="s">
+        <v>22</v>
+      </c>
+      <c r="D118">
+        <f>$F116*D117</f>
+        <v>28723.532941876561</v>
+      </c>
+      <c r="E118">
+        <f t="shared" ref="E118:J118" si="130">$F116*E117</f>
+        <v>3847.7489412005602</v>
+      </c>
+      <c r="F118">
+        <f t="shared" si="130"/>
+        <v>0</v>
+      </c>
+      <c r="G118">
+        <f t="shared" si="130"/>
+        <v>147.92994082876001</v>
+      </c>
+      <c r="H118">
+        <f t="shared" si="130"/>
+        <v>3847.7489412005602</v>
+      </c>
+      <c r="I118">
+        <f t="shared" si="130"/>
+        <v>525.77595857556003</v>
+      </c>
+      <c r="J118">
+        <f t="shared" si="130"/>
+        <v>64.23723903202</v>
+      </c>
+    </row>
+    <row r="119" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A119" s="1">
+        <v>44256</v>
+      </c>
+      <c r="B119" t="s">
+        <v>21</v>
+      </c>
+      <c r="C119" t="s">
+        <v>23</v>
+      </c>
+      <c r="D119">
+        <f>D116-D118</f>
+        <v>1616435.2370581236</v>
+      </c>
+      <c r="E119">
+        <f t="shared" ref="E119:J119" si="131">E116-E118</f>
+        <v>51607.041058799441</v>
+      </c>
+      <c r="F119">
+        <f t="shared" si="131"/>
+        <v>36969.86</v>
+      </c>
+      <c r="G119">
+        <f t="shared" si="131"/>
+        <v>3750.525458847329</v>
+      </c>
+      <c r="H119">
+        <f t="shared" si="131"/>
+        <v>125546.76105879944</v>
+      </c>
+      <c r="I119">
+        <f t="shared" si="131"/>
+        <v>-127.15532269871687</v>
+      </c>
+      <c r="J119">
+        <f t="shared" si="131"/>
+        <v>3202.9554471735728</v>
+      </c>
+    </row>
+    <row r="120" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A120" s="1">
+        <v>44256</v>
+      </c>
+      <c r="B120" t="s">
+        <v>21</v>
+      </c>
+      <c r="C120" t="s">
+        <v>24</v>
+      </c>
+      <c r="D120">
+        <f>D114+D119</f>
+        <v>1765950.4688670384</v>
+      </c>
+      <c r="E120">
+        <f t="shared" ref="E120:J120" si="132">E114+E119</f>
+        <v>157625.82368474605</v>
+      </c>
+      <c r="F120">
+        <f t="shared" si="132"/>
+        <v>63330.508119797552</v>
+      </c>
+      <c r="G120">
+        <f t="shared" si="132"/>
+        <v>26028.992632762445</v>
+      </c>
+      <c r="H120">
+        <f t="shared" si="132"/>
+        <v>130576.63133022525</v>
+      </c>
+      <c r="I120">
+        <f t="shared" si="132"/>
+        <v>-127.15532269871687</v>
+      </c>
+      <c r="J120">
+        <f t="shared" si="132"/>
+        <v>3202.9554471735728</v>
+      </c>
+    </row>
+    <row r="121" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A121" s="1">
+        <v>44256</v>
+      </c>
+      <c r="B121" t="s">
+        <v>21</v>
+      </c>
+      <c r="C121" t="s">
+        <v>25</v>
+      </c>
+      <c r="D121">
+        <f>D120/SUM($D120:$J120)</f>
+        <v>0.82267779562858034</v>
+      </c>
+      <c r="E121">
+        <f t="shared" ref="E121" si="133">E120/SUM($D120:$J120)</f>
+        <v>7.343086199144673E-2</v>
+      </c>
+      <c r="F121">
+        <f t="shared" ref="F121:J121" si="134">F120/SUM($D120:$J120)</f>
+        <v>2.9502867568793466E-2</v>
+      </c>
+      <c r="G121">
+        <f t="shared" si="134"/>
+        <v>1.2125750217270576E-2</v>
+      </c>
+      <c r="H121">
+        <f t="shared" si="134"/>
+        <v>6.0829846089779295E-2</v>
+      </c>
+      <c r="I121">
+        <f t="shared" si="134"/>
+        <v>-5.923601053620338E-5</v>
+      </c>
+      <c r="J121">
+        <f t="shared" si="134"/>
+        <v>1.492114514665758E-3</v>
+      </c>
+    </row>
+    <row r="122" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A122" s="1">
+        <v>44361</v>
+      </c>
+      <c r="B122" t="s">
+        <v>18</v>
+      </c>
+      <c r="C122" t="s">
+        <v>26</v>
+      </c>
+      <c r="D122">
+        <v>0.62</v>
+      </c>
+      <c r="E122">
+        <v>0.46</v>
+      </c>
+      <c r="F122">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="G122">
+        <v>0.86</v>
+      </c>
+      <c r="H122">
+        <v>0.27</v>
+      </c>
+      <c r="O122">
+        <v>469225.79599999997</v>
+      </c>
+      <c r="P122">
+        <v>511877.33199999999</v>
+      </c>
+      <c r="Q122">
+        <v>183840</v>
+      </c>
+      <c r="R122">
+        <v>99881.19</v>
+      </c>
+      <c r="S122">
+        <v>31570.628000000001</v>
+      </c>
+    </row>
+    <row r="123" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A123" s="1">
+        <v>44361</v>
+      </c>
+      <c r="B123" t="s">
+        <v>18</v>
+      </c>
+      <c r="C123" t="s">
+        <v>19</v>
+      </c>
+      <c r="D123">
+        <f>D122*O122</f>
+        <v>290919.99351999996</v>
+      </c>
+      <c r="E123">
+        <f>E122*P122</f>
+        <v>235463.57272</v>
+      </c>
+      <c r="F123">
+        <f>F122*Q122</f>
+        <v>106627.2</v>
+      </c>
+      <c r="G123">
+        <f>G122*R122</f>
+        <v>85897.823399999994</v>
+      </c>
+      <c r="H123">
+        <f>H122*S122</f>
+        <v>8524.0695599999999</v>
+      </c>
+      <c r="K123">
+        <v>987016</v>
+      </c>
+      <c r="L123">
+        <f>K123-(SUM(D123:H123))</f>
+        <v>259583.34080000012</v>
+      </c>
+      <c r="O123">
+        <v>469225.79599999997</v>
+      </c>
+      <c r="P123">
+        <v>511877.33199999999</v>
+      </c>
+      <c r="Q123">
+        <v>183840</v>
+      </c>
+      <c r="R123">
+        <v>99881.19</v>
+      </c>
+      <c r="S123">
+        <v>31570.628000000001</v>
+      </c>
+    </row>
+    <row r="124" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A124" s="1">
+        <v>44361</v>
+      </c>
+      <c r="B124" t="s">
+        <v>18</v>
+      </c>
+      <c r="C124" t="s">
+        <v>20</v>
+      </c>
+      <c r="D124">
+        <f>D123+(D123/(SUM($D123:$H123)))*$L123</f>
+        <v>394734.39182662469</v>
+      </c>
+      <c r="E124">
+        <f t="shared" ref="E124:H124" si="135">E123+(E123/(SUM($D123:$H123)))*$L123</f>
+        <v>319488.42377711541</v>
+      </c>
+      <c r="F124">
+        <f t="shared" si="135"/>
+        <v>144676.96920693881</v>
+      </c>
+      <c r="G124">
+        <f t="shared" si="135"/>
+        <v>116550.34316745508</v>
+      </c>
+      <c r="H124">
+        <f t="shared" si="135"/>
+        <v>11565.872021866133</v>
+      </c>
+    </row>
+    <row r="125" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A125" s="1">
+        <v>44361</v>
+      </c>
+      <c r="B125" t="s">
+        <v>21</v>
+      </c>
+      <c r="C125" t="s">
+        <v>28</v>
+      </c>
+      <c r="D125">
+        <v>0.83</v>
+      </c>
+      <c r="E125">
+        <v>0.05</v>
+      </c>
+      <c r="F125">
+        <v>0.06</v>
+      </c>
+      <c r="G125">
+        <v>0.01</v>
+      </c>
+      <c r="H125">
+        <v>0.1</v>
+      </c>
+      <c r="I125" s="5">
+        <v>2.156462782801142E-4</v>
+      </c>
+      <c r="J125" s="4">
+        <v>1.7674898883607312E-3</v>
+      </c>
+    </row>
+    <row r="126" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A126" s="1">
+        <v>44361</v>
+      </c>
+      <c r="B126" t="s">
+        <v>21</v>
+      </c>
+      <c r="C126" t="s">
+        <v>19</v>
+      </c>
+      <c r="D126">
+        <f>D125*$K126</f>
+        <v>4709524.58</v>
+      </c>
+      <c r="E126">
+        <f t="shared" ref="E126:J126" si="136">E125*$K126</f>
+        <v>283706.3</v>
+      </c>
+      <c r="F126">
+        <f t="shared" si="136"/>
+        <v>340447.56</v>
+      </c>
+      <c r="G126">
+        <f t="shared" si="136"/>
+        <v>56741.26</v>
+      </c>
+      <c r="H126">
+        <f t="shared" si="136"/>
+        <v>567412.6</v>
+      </c>
+      <c r="I126">
+        <f t="shared" si="136"/>
+        <v>1223.6041543924314</v>
+      </c>
+      <c r="J126">
+        <f t="shared" si="136"/>
+        <v>10028.960330284723</v>
+      </c>
+      <c r="K126" s="2">
+        <v>5674126</v>
+      </c>
+    </row>
+    <row r="127" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A127" s="1">
+        <v>44361</v>
+      </c>
+      <c r="B127" t="s">
+        <v>21</v>
+      </c>
+      <c r="C127" t="s">
+        <v>29</v>
+      </c>
+      <c r="D127">
+        <v>0.77694459599999999</v>
+      </c>
+      <c r="E127">
+        <v>0.10407799600000001</v>
+      </c>
+      <c r="G127">
+        <v>4.0013660000000001E-3</v>
+      </c>
+      <c r="H127">
+        <v>0.10407799600000001</v>
+      </c>
+      <c r="I127">
+        <v>1.4221746E-2</v>
+      </c>
+      <c r="J127">
+        <v>1.737557E-3</v>
+      </c>
+      <c r="K127" s="2"/>
+    </row>
+    <row r="128" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A128" s="1">
+        <v>44361</v>
+      </c>
+      <c r="B128" t="s">
+        <v>21</v>
+      </c>
+      <c r="C128" t="s">
+        <v>22</v>
+      </c>
+      <c r="D128">
+        <f>$F126*D127</f>
+        <v>264508.89196338574</v>
+      </c>
+      <c r="E128">
+        <f t="shared" ref="E128:J128" si="137">$F126*E127</f>
+        <v>35433.099787889762</v>
+      </c>
+      <c r="F128">
+        <f t="shared" si="137"/>
+        <v>0</v>
+      </c>
+      <c r="G128">
+        <f t="shared" si="137"/>
+        <v>1362.2552913669601</v>
+      </c>
+      <c r="H128">
+        <f t="shared" si="137"/>
+        <v>35433.099787889762</v>
+      </c>
+      <c r="I128">
+        <f t="shared" si="137"/>
+        <v>4841.7587246397597</v>
+      </c>
+      <c r="J128">
+        <f t="shared" si="137"/>
+        <v>591.54704101092</v>
+      </c>
+    </row>
+    <row r="129" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A129" s="1">
+        <v>44361</v>
+      </c>
+      <c r="B129" t="s">
+        <v>21</v>
+      </c>
+      <c r="C129" t="s">
+        <v>23</v>
+      </c>
+      <c r="D129">
+        <f>D126-D128</f>
+        <v>4445015.6880366141</v>
+      </c>
+      <c r="E129">
+        <f t="shared" ref="E129:J129" si="138">E126-E128</f>
+        <v>248273.20021211024</v>
+      </c>
+      <c r="F129">
+        <f t="shared" si="138"/>
+        <v>340447.56</v>
+      </c>
+      <c r="G129">
+        <f t="shared" si="138"/>
+        <v>55379.004708633045</v>
+      </c>
+      <c r="H129">
+        <f t="shared" si="138"/>
+        <v>531979.50021211023</v>
+      </c>
+      <c r="I129">
+        <f t="shared" si="138"/>
+        <v>-3618.1545702473286</v>
+      </c>
+      <c r="J129">
+        <f t="shared" si="138"/>
+        <v>9437.4132892738035</v>
+      </c>
+    </row>
+    <row r="130" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A130" s="1">
+        <v>44361</v>
+      </c>
+      <c r="B130" t="s">
+        <v>21</v>
+      </c>
+      <c r="C130" t="s">
+        <v>24</v>
+      </c>
+      <c r="D130">
+        <f>D124+D129</f>
+        <v>4839750.0798632391</v>
+      </c>
+      <c r="E130">
+        <f t="shared" ref="E130:J130" si="139">E124+E129</f>
+        <v>567761.6239892256</v>
+      </c>
+      <c r="F130">
+        <f t="shared" si="139"/>
+        <v>485124.52920693881</v>
+      </c>
+      <c r="G130">
+        <f t="shared" si="139"/>
+        <v>171929.34787608811</v>
+      </c>
+      <c r="H130">
+        <f t="shared" si="139"/>
+        <v>543545.37223397638</v>
+      </c>
+      <c r="I130">
+        <f t="shared" si="139"/>
+        <v>-3618.1545702473286</v>
+      </c>
+      <c r="J130">
+        <f t="shared" si="139"/>
+        <v>9437.4132892738035</v>
+      </c>
+    </row>
+    <row r="131" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A131" s="1">
+        <v>44361</v>
+      </c>
+      <c r="B131" t="s">
+        <v>21</v>
+      </c>
+      <c r="C131" t="s">
+        <v>25</v>
+      </c>
+      <c r="D131">
+        <f>D130/SUM($D130:$J130)</f>
+        <v>0.73175100504747104</v>
+      </c>
+      <c r="E131">
+        <f t="shared" ref="E131" si="140">E130/SUM($D130:$J130)</f>
+        <v>8.5843304328896294E-2</v>
+      </c>
+      <c r="F131">
+        <f t="shared" ref="F131:J131" si="141">F130/SUM($D130:$J130)</f>
+        <v>7.3348903551315181E-2</v>
+      </c>
+      <c r="G131">
+        <f t="shared" si="141"/>
+        <v>2.5995035080207871E-2</v>
+      </c>
+      <c r="H131">
+        <f t="shared" si="141"/>
+        <v>8.2181903168097731E-2</v>
+      </c>
+      <c r="I131">
+        <f t="shared" si="141"/>
+        <v>-5.4705061201639534E-4</v>
+      </c>
+      <c r="J131">
+        <f t="shared" si="141"/>
+        <v>1.4268994360282358E-3</v>
+      </c>
+    </row>
+    <row r="132" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A132" s="1">
+        <v>44368</v>
+      </c>
+      <c r="B132" t="s">
+        <v>18</v>
+      </c>
+      <c r="C132" t="s">
+        <v>26</v>
+      </c>
+      <c r="D132">
+        <v>0.62</v>
+      </c>
+      <c r="E132">
+        <v>0.47</v>
+      </c>
+      <c r="F132">
+        <v>0.59</v>
+      </c>
+      <c r="G132">
+        <v>0.87</v>
+      </c>
+      <c r="H132">
+        <v>0.27</v>
+      </c>
+      <c r="O132">
+        <v>469225.79599999997</v>
+      </c>
+      <c r="P132">
+        <v>511877.33199999999</v>
+      </c>
+      <c r="Q132">
+        <v>183840</v>
+      </c>
+      <c r="R132">
+        <v>99881.19</v>
+      </c>
+      <c r="S132">
+        <v>31570.628000000001</v>
+      </c>
+    </row>
+    <row r="133" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A133" s="1">
+        <v>44368</v>
+      </c>
+      <c r="B133" t="s">
+        <v>18</v>
+      </c>
+      <c r="C133" t="s">
+        <v>19</v>
+      </c>
+      <c r="D133">
+        <f>D132*O132</f>
+        <v>290919.99351999996</v>
+      </c>
+      <c r="E133">
+        <f>E132*P132</f>
+        <v>240582.34603999997</v>
+      </c>
+      <c r="F133">
+        <f>F132*Q132</f>
+        <v>108465.59999999999</v>
+      </c>
+      <c r="G133">
+        <f>G132*R132</f>
+        <v>86896.635299999994</v>
+      </c>
+      <c r="H133">
+        <f>H132*S132</f>
+        <v>8524.0695599999999</v>
+      </c>
+      <c r="K133">
+        <v>997393</v>
+      </c>
+      <c r="L133">
+        <f>K133-(SUM(D133:H133))</f>
+        <v>262004.35558000009</v>
+      </c>
+      <c r="O133">
+        <v>469225.79599999997</v>
+      </c>
+      <c r="P133">
+        <v>511877.33199999999</v>
+      </c>
+      <c r="Q133">
+        <v>183840</v>
+      </c>
+      <c r="R133">
+        <v>99881.19</v>
+      </c>
+      <c r="S133">
+        <v>31570.628000000001</v>
+      </c>
+    </row>
+    <row r="134" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A134" s="1">
+        <v>44368</v>
+      </c>
+      <c r="B134" t="s">
+        <v>18</v>
+      </c>
+      <c r="C134" t="s">
+        <v>20</v>
+      </c>
+      <c r="D134">
+        <f>D133+(D133/(SUM($D133:$H133)))*$L133</f>
+        <v>394569.00415662985</v>
+      </c>
+      <c r="E134">
+        <f t="shared" ref="E134:H134" si="142">E133+(E133/(SUM($D133:$H133)))*$L133</f>
+        <v>326297.05351668305</v>
+      </c>
+      <c r="F134">
+        <f t="shared" si="142"/>
+        <v>147109.73714602794</v>
+      </c>
+      <c r="G134">
+        <f t="shared" si="142"/>
+        <v>117856.1790821906</v>
+      </c>
+      <c r="H134">
+        <f t="shared" si="142"/>
+        <v>11561.026098468621</v>
+      </c>
+    </row>
+    <row r="135" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A135" s="1">
+        <v>44368</v>
+      </c>
+      <c r="B135" t="s">
+        <v>21</v>
+      </c>
+      <c r="C135" t="s">
+        <v>28</v>
+      </c>
+      <c r="D135">
+        <v>0.85</v>
+      </c>
+      <c r="E135">
+        <v>0.05</v>
+      </c>
+      <c r="F135">
+        <v>0.05</v>
+      </c>
+      <c r="G135">
+        <v>0.01</v>
+      </c>
+      <c r="H135">
+        <v>0.09</v>
+      </c>
+      <c r="I135" s="5">
+        <v>2.156462782801142E-4</v>
+      </c>
+      <c r="J135" s="4">
+        <v>1.7674898883607312E-3</v>
+      </c>
+    </row>
+    <row r="136" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A136" s="1">
+        <v>44368</v>
+      </c>
+      <c r="B136" t="s">
+        <v>21</v>
+      </c>
+      <c r="C136" t="s">
+        <v>19</v>
+      </c>
+      <c r="D136">
+        <f>D135*$K136</f>
+        <v>4865507.95</v>
+      </c>
+      <c r="E136">
+        <f t="shared" ref="E136:J136" si="143">E135*$K136</f>
+        <v>286206.35000000003</v>
+      </c>
+      <c r="F136">
+        <f t="shared" si="143"/>
+        <v>286206.35000000003</v>
+      </c>
+      <c r="G136">
+        <f t="shared" si="143"/>
+        <v>57241.270000000004</v>
+      </c>
+      <c r="H136">
+        <f t="shared" si="143"/>
+        <v>515171.43</v>
+      </c>
+      <c r="I136">
+        <f t="shared" si="143"/>
+        <v>1234.3866839527152</v>
+      </c>
+      <c r="J136">
+        <f t="shared" si="143"/>
+        <v>10117.336592192647</v>
+      </c>
+      <c r="K136" s="2">
+        <v>5724127</v>
+      </c>
+    </row>
+    <row r="137" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A137" s="1">
+        <v>44368</v>
+      </c>
+      <c r="B137" t="s">
+        <v>21</v>
+      </c>
+      <c r="C137" t="s">
+        <v>29</v>
+      </c>
+      <c r="D137">
+        <v>0.77694459599999999</v>
+      </c>
+      <c r="E137">
+        <v>0.10407799600000001</v>
+      </c>
+      <c r="G137">
+        <v>4.0013660000000001E-3</v>
+      </c>
+      <c r="H137">
+        <v>0.10407799600000001</v>
+      </c>
+      <c r="I137">
+        <v>1.4221746E-2</v>
+      </c>
+      <c r="J137">
+        <v>1.737557E-3</v>
+      </c>
+      <c r="K137" s="2"/>
+    </row>
+    <row r="138" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A138" s="1">
+        <v>44368</v>
+      </c>
+      <c r="B138" t="s">
+        <v>21</v>
+      </c>
+      <c r="C138" t="s">
+        <v>22</v>
+      </c>
+      <c r="D138">
+        <f>$F136*D137</f>
+        <v>222366.47697338462</v>
+      </c>
+      <c r="E138">
+        <f t="shared" ref="E138:J138" si="144">$F136*E137</f>
+        <v>29787.783350474605</v>
+      </c>
+      <c r="F138">
+        <f t="shared" si="144"/>
+        <v>0</v>
+      </c>
+      <c r="G138">
+        <f t="shared" si="144"/>
+        <v>1145.2163578741001</v>
+      </c>
+      <c r="H138">
+        <f t="shared" si="144"/>
+        <v>29787.783350474605</v>
+      </c>
+      <c r="I138">
+        <f t="shared" si="144"/>
+        <v>4070.3540132871008</v>
+      </c>
+      <c r="J138">
+        <f t="shared" si="144"/>
+        <v>497.29984688695009</v>
+      </c>
+    </row>
+    <row r="139" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A139" s="1">
+        <v>44368</v>
+      </c>
+      <c r="B139" t="s">
+        <v>21</v>
+      </c>
+      <c r="C139" t="s">
+        <v>23</v>
+      </c>
+      <c r="D139">
+        <f>D136-D138</f>
+        <v>4643141.4730266156</v>
+      </c>
+      <c r="E139">
+        <f t="shared" ref="E139:J139" si="145">E136-E138</f>
+        <v>256418.56664952543</v>
+      </c>
+      <c r="F139">
+        <f t="shared" si="145"/>
+        <v>286206.35000000003</v>
+      </c>
+      <c r="G139">
+        <f t="shared" si="145"/>
+        <v>56096.053642125902</v>
+      </c>
+      <c r="H139">
+        <f t="shared" si="145"/>
+        <v>485383.64664952538</v>
+      </c>
+      <c r="I139">
+        <f t="shared" si="145"/>
+        <v>-2835.9673293343858</v>
+      </c>
+      <c r="J139">
+        <f t="shared" si="145"/>
+        <v>9620.036745305697</v>
+      </c>
+    </row>
+    <row r="140" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A140" s="1">
+        <v>44368</v>
+      </c>
+      <c r="B140" t="s">
+        <v>21</v>
+      </c>
+      <c r="C140" t="s">
+        <v>24</v>
+      </c>
+      <c r="D140">
+        <f>D134+D139</f>
+        <v>5037710.4771832451</v>
+      </c>
+      <c r="E140">
+        <f t="shared" ref="E140:J140" si="146">E134+E139</f>
+        <v>582715.62016620848</v>
+      </c>
+      <c r="F140">
+        <f t="shared" si="146"/>
+        <v>433316.08714602794</v>
+      </c>
+      <c r="G140">
+        <f t="shared" si="146"/>
+        <v>173952.23272431651</v>
+      </c>
+      <c r="H140">
+        <f t="shared" si="146"/>
+        <v>496944.67274799402</v>
+      </c>
+      <c r="I140">
+        <f t="shared" si="146"/>
+        <v>-2835.9673293343858</v>
+      </c>
+      <c r="J140">
+        <f t="shared" si="146"/>
+        <v>9620.036745305697</v>
+      </c>
+    </row>
+    <row r="141" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A141" s="1">
+        <v>44368</v>
+      </c>
+      <c r="B141" t="s">
+        <v>21</v>
+      </c>
+      <c r="C141" t="s">
+        <v>25</v>
+      </c>
+      <c r="D141">
+        <f>D140/SUM($D140:$J140)</f>
+        <v>0.7483871326913325</v>
+      </c>
+      <c r="E141">
+        <f t="shared" ref="E141" si="147">E140/SUM($D140:$J140)</f>
+        <v>8.6566481763056161E-2</v>
+      </c>
+      <c r="F141">
+        <f t="shared" ref="F141:J141" si="148">F140/SUM($D140:$J140)</f>
+        <v>6.4372136008412281E-2</v>
+      </c>
+      <c r="G141">
+        <f t="shared" si="148"/>
+        <v>2.5841821054114384E-2</v>
+      </c>
+      <c r="H141">
+        <f t="shared" si="148"/>
+        <v>7.3824607513381671E-2</v>
+      </c>
+      <c r="I141">
+        <f t="shared" si="148"/>
+        <v>-4.2130278578326785E-4</v>
+      </c>
+      <c r="J141">
+        <f t="shared" si="148"/>
+        <v>1.4291237554862582E-3</v>
+      </c>
+    </row>
+    <row r="142" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A142" s="1">
+        <v>44375</v>
+      </c>
+      <c r="B142" t="s">
+        <v>18</v>
+      </c>
+      <c r="C142" t="s">
+        <v>26</v>
+      </c>
+      <c r="D142">
+        <v>0.62</v>
+      </c>
+      <c r="E142">
+        <v>0.48</v>
+      </c>
+      <c r="F142">
+        <v>0.61</v>
+      </c>
+      <c r="G142">
+        <v>0.88</v>
+      </c>
+      <c r="H142">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="O142">
+        <v>469225.79599999997</v>
+      </c>
+      <c r="P142">
+        <v>511877.33199999999</v>
+      </c>
+      <c r="Q142">
+        <v>183840</v>
+      </c>
+      <c r="R142">
+        <v>99881.19</v>
+      </c>
+      <c r="S142">
+        <v>31570.628000000001</v>
+      </c>
+    </row>
+    <row r="143" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A143" s="1">
+        <v>44375</v>
+      </c>
+      <c r="B143" t="s">
+        <v>18</v>
+      </c>
+      <c r="C143" t="s">
+        <v>19</v>
+      </c>
+      <c r="D143">
+        <f>D142*O142</f>
+        <v>290919.99351999996</v>
+      </c>
+      <c r="E143">
+        <f>E142*P142</f>
+        <v>245701.11935999998</v>
+      </c>
+      <c r="F143">
+        <f>F142*Q142</f>
+        <v>112142.39999999999</v>
+      </c>
+      <c r="G143">
+        <f>G142*R142</f>
+        <v>87895.44720000001</v>
+      </c>
+      <c r="H143">
+        <f>H142*S142</f>
+        <v>8839.7758400000002</v>
+      </c>
+      <c r="K143">
+        <v>1006006</v>
+      </c>
+      <c r="L143">
+        <f>K143-(SUM(D143:H143))</f>
+        <v>260507.26407999999</v>
+      </c>
+      <c r="O143">
+        <v>469225.79599999997</v>
+      </c>
+      <c r="P143">
+        <v>511877.33199999999</v>
+      </c>
+      <c r="Q143">
+        <v>183840</v>
+      </c>
+      <c r="R143">
+        <v>99881.19</v>
+      </c>
+      <c r="S143">
+        <v>31570.628000000001</v>
+      </c>
+    </row>
+    <row r="144" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A144" s="1">
+        <v>44375</v>
+      </c>
+      <c r="B144" t="s">
+        <v>18</v>
+      </c>
+      <c r="C144" t="s">
+        <v>20</v>
+      </c>
+      <c r="D144">
+        <f>D143+(D143/(SUM($D143:$H143)))*$L143</f>
+        <v>392579.14856141002</v>
+      </c>
+      <c r="E144">
+        <f t="shared" ref="E144:H144" si="149">E143+(E143/(SUM($D143:$H143)))*$L143</f>
+        <v>331558.97974507208</v>
+      </c>
+      <c r="F144">
+        <f t="shared" si="149"/>
+        <v>151329.46820516989</v>
+      </c>
+      <c r="G144">
+        <f t="shared" si="149"/>
+        <v>118609.65417568728</v>
+      </c>
+      <c r="H144">
+        <f t="shared" si="149"/>
+        <v>11928.749312660591</v>
+      </c>
+    </row>
+    <row r="145" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A145" s="1">
+        <v>44375</v>
+      </c>
+      <c r="B145" t="s">
+        <v>21</v>
+      </c>
+      <c r="C145" t="s">
+        <v>28</v>
+      </c>
+      <c r="D145">
+        <v>0.84</v>
+      </c>
+      <c r="E145">
+        <v>0.05</v>
+      </c>
+      <c r="F145">
+        <v>0.06</v>
+      </c>
+      <c r="G145">
+        <v>0.01</v>
+      </c>
+      <c r="H145">
+        <v>0.09</v>
+      </c>
+      <c r="I145" s="5">
+        <v>2.156462782801142E-4</v>
+      </c>
+      <c r="J145" s="4">
+        <v>1.7674898883607312E-3</v>
+      </c>
+    </row>
+    <row r="146" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A146" s="1">
+        <v>44375</v>
+      </c>
+      <c r="B146" t="s">
+        <v>21</v>
+      </c>
+      <c r="C146" t="s">
+        <v>19</v>
+      </c>
+      <c r="D146">
+        <f>D145*$K146</f>
+        <v>4845239.28</v>
+      </c>
+      <c r="E146">
+        <f t="shared" ref="E146:J146" si="150">E145*$K146</f>
+        <v>288407.10000000003</v>
+      </c>
+      <c r="F146">
+        <f t="shared" si="150"/>
+        <v>346088.51999999996</v>
+      </c>
+      <c r="G146">
+        <f t="shared" si="150"/>
+        <v>57681.42</v>
+      </c>
+      <c r="H146">
+        <f t="shared" si="150"/>
+        <v>519132.77999999997</v>
+      </c>
+      <c r="I146">
+        <f t="shared" si="150"/>
+        <v>1243.8783548912145</v>
+      </c>
+      <c r="J146">
+        <f t="shared" si="150"/>
+        <v>10195.132659628845</v>
+      </c>
+      <c r="K146" s="2">
+        <v>5768142</v>
+      </c>
+    </row>
+    <row r="147" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A147" s="1">
+        <v>44375</v>
+      </c>
+      <c r="B147" t="s">
+        <v>21</v>
+      </c>
+      <c r="C147" t="s">
+        <v>29</v>
+      </c>
+      <c r="D147">
+        <v>0.77694459599999999</v>
+      </c>
+      <c r="E147">
+        <v>0.10407799600000001</v>
+      </c>
+      <c r="G147">
+        <v>4.0013660000000001E-3</v>
+      </c>
+      <c r="H147">
+        <v>0.10407799600000001</v>
+      </c>
+      <c r="I147">
+        <v>1.4221746E-2</v>
+      </c>
+      <c r="J147">
+        <v>1.737557E-3</v>
+      </c>
+      <c r="K147" s="2"/>
+    </row>
+    <row r="148" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A148" s="1">
+        <v>44375</v>
+      </c>
+      <c r="B148" t="s">
+        <v>21</v>
+      </c>
+      <c r="C148" t="s">
+        <v>22</v>
+      </c>
+      <c r="D148">
+        <f>$F146*D147</f>
+        <v>268891.60535163787</v>
+      </c>
+      <c r="E148">
+        <f t="shared" ref="E148:J148" si="151">$F146*E147</f>
+        <v>36020.199600205917</v>
+      </c>
+      <c r="F148">
+        <f t="shared" si="151"/>
+        <v>0</v>
+      </c>
+      <c r="G148">
+        <f t="shared" si="151"/>
+        <v>1384.8268369183199</v>
+      </c>
+      <c r="H148">
+        <f t="shared" si="151"/>
+        <v>36020.199600205917</v>
+      </c>
+      <c r="I148">
+        <f t="shared" si="151"/>
+        <v>4921.98302495592</v>
+      </c>
+      <c r="J148">
+        <f t="shared" si="151"/>
+        <v>601.34853054563996</v>
+      </c>
+    </row>
+    <row r="149" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A149" s="1">
+        <v>44375</v>
+      </c>
+      <c r="B149" t="s">
+        <v>21</v>
+      </c>
+      <c r="C149" t="s">
+        <v>23</v>
+      </c>
+      <c r="D149">
+        <f>D146-D148</f>
+        <v>4576347.6746483622</v>
+      </c>
+      <c r="E149">
+        <f t="shared" ref="E149:J149" si="152">E146-E148</f>
+        <v>252386.9003997941</v>
+      </c>
+      <c r="F149">
+        <f t="shared" si="152"/>
+        <v>346088.51999999996</v>
+      </c>
+      <c r="G149">
+        <f t="shared" si="152"/>
+        <v>56296.593163081678</v>
+      </c>
+      <c r="H149">
+        <f t="shared" si="152"/>
+        <v>483112.58039979404</v>
+      </c>
+      <c r="I149">
+        <f t="shared" si="152"/>
+        <v>-3678.1046700647057</v>
+      </c>
+      <c r="J149">
+        <f t="shared" si="152"/>
+        <v>9593.7841290832057</v>
+      </c>
+    </row>
+    <row r="150" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A150" s="1">
+        <v>44375</v>
+      </c>
+      <c r="B150" t="s">
+        <v>21</v>
+      </c>
+      <c r="C150" t="s">
+        <v>24</v>
+      </c>
+      <c r="D150">
+        <f>D144+D149</f>
+        <v>4968926.8232097719</v>
+      </c>
+      <c r="E150">
+        <f t="shared" ref="E150:J150" si="153">E144+E149</f>
+        <v>583945.88014486618</v>
+      </c>
+      <c r="F150">
+        <f t="shared" si="153"/>
+        <v>497417.98820516985</v>
+      </c>
+      <c r="G150">
+        <f t="shared" si="153"/>
+        <v>174906.24733876897</v>
+      </c>
+      <c r="H150">
+        <f t="shared" si="153"/>
+        <v>495041.32971245464</v>
+      </c>
+      <c r="I150">
+        <f t="shared" si="153"/>
+        <v>-3678.1046700647057</v>
+      </c>
+      <c r="J150">
+        <f t="shared" si="153"/>
+        <v>9593.7841290832057</v>
+      </c>
+    </row>
+    <row r="151" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A151" s="1">
+        <v>44375</v>
+      </c>
+      <c r="B151" t="s">
+        <v>21</v>
+      </c>
+      <c r="C151" t="s">
+        <v>25</v>
+      </c>
+      <c r="D151">
+        <f>D150/SUM($D150:$J150)</f>
+        <v>0.73874711485536493</v>
+      </c>
+      <c r="E151">
+        <f t="shared" ref="E151" si="154">E150/SUM($D150:$J150)</f>
+        <v>8.6817204104051027E-2</v>
+      </c>
+      <c r="F151">
+        <f t="shared" ref="F151:J151" si="155">F150/SUM($D150:$J150)</f>
+        <v>7.3952810483604095E-2</v>
+      </c>
+      <c r="G151">
+        <f t="shared" si="155"/>
+        <v>2.6003901886449566E-2</v>
+      </c>
+      <c r="H151">
+        <f t="shared" si="155"/>
+        <v>7.359946464717744E-2</v>
+      </c>
+      <c r="I151">
+        <f t="shared" si="155"/>
+        <v>-5.4683623040178444E-4</v>
+      </c>
+      <c r="J151">
+        <f t="shared" si="155"/>
+        <v>1.4263402537546693E-3</v>
+      </c>
+    </row>
+    <row r="152" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A152" s="1">
+        <v>44383</v>
+      </c>
+      <c r="B152" t="s">
+        <v>18</v>
+      </c>
+      <c r="C152" t="s">
+        <v>26</v>
+      </c>
+      <c r="D152">
+        <v>0.63</v>
+      </c>
+      <c r="E152">
+        <v>0.48</v>
+      </c>
+      <c r="F152">
+        <v>0.62</v>
+      </c>
+      <c r="G152">
+        <v>0.89</v>
+      </c>
+      <c r="H152">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="O152">
+        <v>469225.79599999997</v>
+      </c>
+      <c r="P152">
+        <v>511877.33199999999</v>
+      </c>
+      <c r="Q152">
+        <v>183840</v>
+      </c>
+      <c r="R152">
+        <v>99881.19</v>
+      </c>
+      <c r="S152">
+        <v>31570.628000000001</v>
+      </c>
+    </row>
+    <row r="153" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A153" s="1">
+        <v>44383</v>
+      </c>
+      <c r="B153" t="s">
+        <v>18</v>
+      </c>
+      <c r="C153" t="s">
+        <v>19</v>
+      </c>
+      <c r="D153">
+        <f>D152*O152</f>
+        <v>295612.25147999998</v>
+      </c>
+      <c r="E153">
+        <f>E152*P152</f>
+        <v>245701.11935999998</v>
+      </c>
+      <c r="F153">
+        <f>F152*Q152</f>
+        <v>113980.8</v>
+      </c>
+      <c r="G153">
+        <f>G152*R152</f>
+        <v>88894.25910000001</v>
+      </c>
+      <c r="H153">
+        <f>H152*S152</f>
+        <v>8839.7758400000002</v>
+      </c>
+      <c r="K153">
+        <v>1013376</v>
+      </c>
+      <c r="L153">
+        <f>K153-(SUM(D153:H153))</f>
+        <v>260347.79421999992</v>
+      </c>
+      <c r="O153">
+        <v>469225.79599999997</v>
+      </c>
+      <c r="P153">
+        <v>511877.33199999999</v>
+      </c>
+      <c r="Q153">
+        <v>183840</v>
+      </c>
+      <c r="R153">
+        <v>99881.19</v>
+      </c>
+      <c r="S153">
+        <v>31570.628000000001</v>
+      </c>
+    </row>
+    <row r="154" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A154" s="1">
+        <v>44383</v>
+      </c>
+      <c r="B154" t="s">
+        <v>18</v>
+      </c>
+      <c r="C154" t="s">
+        <v>20</v>
+      </c>
+      <c r="D154">
+        <f>D153+(D153/(SUM($D153:$H153)))*$L153</f>
+        <v>397815.59131042147</v>
+      </c>
+      <c r="E154">
+        <f t="shared" ref="E154:H154" si="156">E153+(E153/(SUM($D153:$H153)))*$L153</f>
+        <v>330648.46126799926</v>
+      </c>
+      <c r="F154">
+        <f t="shared" si="156"/>
+        <v>153387.88944984795</v>
+      </c>
+      <c r="G154">
+        <f t="shared" si="156"/>
+        <v>119628.06707407687</v>
+      </c>
+      <c r="H154">
+        <f t="shared" si="156"/>
+        <v>11895.990897654314</v>
+      </c>
+    </row>
+    <row r="155" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A155" s="1">
+        <v>44383</v>
+      </c>
+      <c r="B155" t="s">
+        <v>21</v>
+      </c>
+      <c r="C155" t="s">
+        <v>28</v>
+      </c>
+      <c r="D155">
+        <v>0.84</v>
+      </c>
+      <c r="E155">
+        <v>0.05</v>
+      </c>
+      <c r="F155">
+        <v>0.06</v>
+      </c>
+      <c r="G155">
+        <v>0.01</v>
+      </c>
+      <c r="H155">
+        <v>0.09</v>
+      </c>
+      <c r="I155" s="5">
+        <v>2.156462782801142E-4</v>
+      </c>
+      <c r="J155" s="4">
+        <v>1.7674898883607312E-3</v>
+      </c>
+    </row>
+    <row r="156" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A156" s="1">
+        <v>44383</v>
+      </c>
+      <c r="B156" t="s">
+        <v>21</v>
+      </c>
+      <c r="C156" t="s">
+        <v>19</v>
+      </c>
+      <c r="D156">
+        <f>D155*$K156</f>
+        <v>4878947.6399999997</v>
+      </c>
+      <c r="E156">
+        <f t="shared" ref="E156:J156" si="157">E155*$K156</f>
+        <v>290413.55</v>
+      </c>
+      <c r="F156">
+        <f t="shared" si="157"/>
+        <v>348496.26</v>
+      </c>
+      <c r="G156">
+        <f t="shared" si="157"/>
+        <v>58082.71</v>
+      </c>
+      <c r="H156">
+        <f t="shared" si="157"/>
+        <v>522744.38999999996</v>
+      </c>
+      <c r="I156">
+        <f t="shared" si="157"/>
+        <v>1252.5320243923172</v>
+      </c>
+      <c r="J156">
+        <f t="shared" si="157"/>
+        <v>10266.060261358873</v>
+      </c>
+      <c r="K156" s="2">
+        <v>5808271</v>
+      </c>
+    </row>
+    <row r="157" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A157" s="1">
+        <v>44383</v>
+      </c>
+      <c r="B157" t="s">
+        <v>21</v>
+      </c>
+      <c r="C157" t="s">
+        <v>29</v>
+      </c>
+      <c r="D157">
+        <v>0.77694459599999999</v>
+      </c>
+      <c r="E157">
+        <v>0.10407799600000001</v>
+      </c>
+      <c r="G157">
+        <v>4.0013660000000001E-3</v>
+      </c>
+      <c r="H157">
+        <v>0.10407799600000001</v>
+      </c>
+      <c r="I157">
+        <v>1.4221746E-2</v>
+      </c>
+      <c r="J157">
+        <v>1.737557E-3</v>
+      </c>
+      <c r="K157" s="2"/>
+    </row>
+    <row r="158" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A158" s="1">
+        <v>44383</v>
+      </c>
+      <c r="B158" t="s">
+        <v>21</v>
+      </c>
+      <c r="C158" t="s">
+        <v>22</v>
+      </c>
+      <c r="D158">
+        <f>$F156*D157</f>
+        <v>270762.28593321098</v>
+      </c>
+      <c r="E158">
+        <f t="shared" ref="E158:J158" si="158">$F156*E157</f>
+        <v>36270.792354294965</v>
+      </c>
+      <c r="F158">
+        <f t="shared" si="158"/>
+        <v>0</v>
+      </c>
+      <c r="G158">
+        <f t="shared" si="158"/>
+        <v>1394.4610858911601</v>
+      </c>
+      <c r="H158">
+        <f t="shared" si="158"/>
+        <v>36270.792354294965</v>
+      </c>
+      <c r="I158">
+        <f t="shared" si="158"/>
+        <v>4956.2252916699599</v>
+      </c>
+      <c r="J158">
+        <f t="shared" si="158"/>
+        <v>605.53211603682007</v>
+      </c>
+    </row>
+    <row r="159" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A159" s="1">
+        <v>44383</v>
+      </c>
+      <c r="B159" t="s">
+        <v>21</v>
+      </c>
+      <c r="C159" t="s">
+        <v>23</v>
+      </c>
+      <c r="D159">
+        <f>D156-D158</f>
+        <v>4608185.3540667892</v>
+      </c>
+      <c r="E159">
+        <f t="shared" ref="E159:J159" si="159">E156-E158</f>
+        <v>254142.75764570502</v>
+      </c>
+      <c r="F159">
+        <f t="shared" si="159"/>
+        <v>348496.26</v>
+      </c>
+      <c r="G159">
+        <f t="shared" si="159"/>
+        <v>56688.248914108837</v>
+      </c>
+      <c r="H159">
+        <f t="shared" si="159"/>
+        <v>486473.59764570498</v>
+      </c>
+      <c r="I159">
+        <f t="shared" si="159"/>
+        <v>-3703.6932672776429</v>
+      </c>
+      <c r="J159">
+        <f t="shared" si="159"/>
+        <v>9660.5281453220523</v>
+      </c>
+    </row>
+    <row r="160" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A160" s="1">
+        <v>44383</v>
+      </c>
+      <c r="B160" t="s">
+        <v>21</v>
+      </c>
+      <c r="C160" t="s">
+        <v>24</v>
+      </c>
+      <c r="D160">
+        <f>D154+D159</f>
+        <v>5006000.9453772102</v>
+      </c>
+      <c r="E160">
+        <f t="shared" ref="E160:J160" si="160">E154+E159</f>
+        <v>584791.21891370427</v>
+      </c>
+      <c r="F160">
+        <f t="shared" si="160"/>
+        <v>501884.14944984799</v>
+      </c>
+      <c r="G160">
+        <f t="shared" si="160"/>
+        <v>176316.3159881857</v>
+      </c>
+      <c r="H160">
+        <f t="shared" si="160"/>
+        <v>498369.58854335931</v>
+      </c>
+      <c r="I160">
+        <f t="shared" si="160"/>
+        <v>-3703.6932672776429</v>
+      </c>
+      <c r="J160">
+        <f t="shared" si="160"/>
+        <v>9660.5281453220523</v>
+      </c>
+    </row>
+    <row r="161" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A161" s="1">
+        <v>44383</v>
+      </c>
+      <c r="B161" t="s">
+        <v>21</v>
+      </c>
+      <c r="C161" t="s">
+        <v>25</v>
+      </c>
+      <c r="D161">
+        <f>D160/SUM($D160:$J160)</f>
+        <v>0.73907650091410648</v>
+      </c>
+      <c r="E161">
+        <f t="shared" ref="E161" si="161">E160/SUM($D160:$J160)</f>
+        <v>8.6337468281774049E-2</v>
+      </c>
+      <c r="F161">
+        <f t="shared" ref="F161:J161" si="162">F160/SUM($D160:$J160)</f>
+        <v>7.4097225527330751E-2</v>
+      </c>
+      <c r="G161">
+        <f t="shared" si="162"/>
+        <v>2.6031007044645105E-2</v>
+      </c>
+      <c r="H161">
+        <f t="shared" si="162"/>
+        <v>7.357834240977644E-2</v>
+      </c>
+      <c r="I161">
+        <f t="shared" si="162"/>
+        <v>-5.4680626118667943E-4</v>
+      </c>
+      <c r="J161">
+        <f t="shared" si="162"/>
+        <v>1.4262620835539743E-3</v>
+      </c>
+    </row>
+    <row r="162" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A162" s="1">
+        <v>44396</v>
+      </c>
+      <c r="B162" t="s">
+        <v>18</v>
+      </c>
+      <c r="C162" t="s">
+        <v>26</v>
+      </c>
+      <c r="D162">
+        <v>0.63</v>
+      </c>
+      <c r="E162">
+        <v>0.5</v>
+      </c>
+      <c r="F162">
+        <v>0.63</v>
+      </c>
+      <c r="G162">
+        <v>0.9</v>
+      </c>
+      <c r="H162">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="O162">
+        <v>469225.79599999997</v>
+      </c>
+      <c r="P162">
+        <v>511877.33199999999</v>
+      </c>
+      <c r="Q162">
+        <v>183840</v>
+      </c>
+      <c r="R162">
+        <v>99881.19</v>
+      </c>
+      <c r="S162">
+        <v>31570.628000000001</v>
+      </c>
+    </row>
+    <row r="163" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A163" s="1">
+        <v>44396</v>
+      </c>
+      <c r="B163" t="s">
+        <v>18</v>
+      </c>
+      <c r="C163" t="s">
+        <v>19</v>
+      </c>
+      <c r="D163">
+        <f>D162*O162</f>
+        <v>295612.25147999998</v>
+      </c>
+      <c r="E163">
+        <f>E162*P162</f>
+        <v>255938.666</v>
+      </c>
+      <c r="F163">
+        <f>F162*Q162</f>
+        <v>115819.2</v>
+      </c>
+      <c r="G163">
+        <f>G162*R162</f>
+        <v>89893.071000000011</v>
+      </c>
+      <c r="H163">
+        <f>H162*S162</f>
+        <v>9155.4821199999988</v>
+      </c>
+      <c r="K163">
+        <v>1031752</v>
+      </c>
+      <c r="L163">
+        <f>K163-(SUM(D163:H163))</f>
+        <v>265333.32940000016</v>
+      </c>
+      <c r="O163">
+        <v>469225.79599999997</v>
+      </c>
+      <c r="P163">
+        <v>511877.33199999999</v>
+      </c>
+      <c r="Q163">
+        <v>183840</v>
+      </c>
+      <c r="R163">
+        <v>99881.19</v>
+      </c>
+      <c r="S163">
+        <v>31570.628000000001</v>
+      </c>
+    </row>
+    <row r="164" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A164" s="1">
+        <v>44396</v>
+      </c>
+      <c r="B164" t="s">
+        <v>18</v>
+      </c>
+      <c r="C164" t="s">
+        <v>20</v>
+      </c>
+      <c r="D164">
+        <f>D163+(D163/(SUM($D163:$H163)))*$L163</f>
+        <v>397952.89883820451</v>
+      </c>
+      <c r="E164">
+        <f t="shared" ref="E164:H164" si="163">E163+(E163/(SUM($D163:$H163)))*$L163</f>
+        <v>344544.36022038118</v>
+      </c>
+      <c r="F164">
+        <f t="shared" si="163"/>
+        <v>155915.68397577084</v>
+      </c>
+      <c r="G164">
+        <f t="shared" si="163"/>
+        <v>121013.95666389971</v>
+      </c>
+      <c r="H164">
+        <f t="shared" si="163"/>
+        <v>12325.100301743929</v>
+      </c>
+    </row>
+    <row r="165" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A165" s="1">
+        <v>44396</v>
+      </c>
+      <c r="B165" t="s">
+        <v>21</v>
+      </c>
+      <c r="C165" t="s">
+        <v>28</v>
+      </c>
+      <c r="D165">
+        <v>0.83</v>
+      </c>
+      <c r="E165">
+        <v>0.05</v>
+      </c>
+      <c r="F165">
+        <v>0.06</v>
+      </c>
+      <c r="G165">
+        <v>0.01</v>
+      </c>
+      <c r="H165">
+        <v>0.1</v>
+      </c>
+      <c r="I165" s="5">
+        <v>2.156462782801142E-4</v>
+      </c>
+      <c r="J165" s="4">
+        <v>1.7674898883607312E-3</v>
+      </c>
+    </row>
+    <row r="166" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A166" s="1">
+        <v>44396</v>
+      </c>
+      <c r="B166" t="s">
+        <v>21</v>
+      </c>
+      <c r="C166" t="s">
+        <v>19</v>
+      </c>
+      <c r="D166">
+        <f>D165*$K166</f>
+        <v>4876706.5</v>
+      </c>
+      <c r="E166">
+        <f t="shared" ref="E166:J166" si="164">E165*$K166</f>
+        <v>293777.5</v>
+      </c>
+      <c r="F166">
+        <f t="shared" si="164"/>
+        <v>352533</v>
+      </c>
+      <c r="G166">
+        <f t="shared" si="164"/>
+        <v>58755.5</v>
+      </c>
+      <c r="H166">
+        <f t="shared" si="164"/>
+        <v>587555</v>
+      </c>
+      <c r="I166">
+        <f t="shared" si="164"/>
+        <v>1267.0404903487249</v>
+      </c>
+      <c r="J166">
+        <f t="shared" si="164"/>
+        <v>10384.975213557895</v>
+      </c>
+      <c r="K166" s="2">
+        <v>5875550</v>
+      </c>
+    </row>
+    <row r="167" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A167" s="1">
+        <v>44396</v>
+      </c>
+      <c r="B167" t="s">
+        <v>21</v>
+      </c>
+      <c r="C167" t="s">
+        <v>29</v>
+      </c>
+      <c r="D167">
+        <v>0.77694459599999999</v>
+      </c>
+      <c r="E167">
+        <v>0.10407799600000001</v>
+      </c>
+      <c r="G167">
+        <v>4.0013660000000001E-3</v>
+      </c>
+      <c r="H167">
+        <v>0.10407799600000001</v>
+      </c>
+      <c r="I167">
+        <v>1.4221746E-2</v>
+      </c>
+      <c r="J167">
+        <v>1.737557E-3</v>
+      </c>
+      <c r="K167" s="2"/>
+    </row>
+    <row r="168" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A168" s="1">
+        <v>44396</v>
+      </c>
+      <c r="B168" t="s">
+        <v>21</v>
+      </c>
+      <c r="C168" t="s">
+        <v>22</v>
+      </c>
+      <c r="D168">
+        <f>$F166*D167</f>
+        <v>273898.609261668</v>
+      </c>
+      <c r="E168">
+        <f t="shared" ref="E168:J168" si="165">$F166*E167</f>
+        <v>36690.928163868004</v>
+      </c>
+      <c r="F168">
+        <f t="shared" si="165"/>
+        <v>0</v>
+      </c>
+      <c r="G168">
+        <f t="shared" si="165"/>
+        <v>1410.6135600780001</v>
+      </c>
+      <c r="H168">
+        <f t="shared" si="165"/>
+        <v>36690.928163868004</v>
+      </c>
+      <c r="I168">
+        <f t="shared" si="165"/>
+        <v>5013.6347826179999</v>
+      </c>
+      <c r="J168">
+        <f t="shared" si="165"/>
+        <v>612.54618188100005</v>
+      </c>
+    </row>
+    <row r="169" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A169" s="1">
+        <v>44396</v>
+      </c>
+      <c r="B169" t="s">
+        <v>21</v>
+      </c>
+      <c r="C169" t="s">
+        <v>23</v>
+      </c>
+      <c r="D169">
+        <f>D166-D168</f>
+        <v>4602807.8907383317</v>
+      </c>
+      <c r="E169">
+        <f t="shared" ref="E169:J169" si="166">E166-E168</f>
+        <v>257086.571836132</v>
+      </c>
+      <c r="F169">
+        <f t="shared" si="166"/>
+        <v>352533</v>
+      </c>
+      <c r="G169">
+        <f t="shared" si="166"/>
+        <v>57344.886439921996</v>
+      </c>
+      <c r="H169">
+        <f t="shared" si="166"/>
+        <v>550864.07183613197</v>
+      </c>
+      <c r="I169">
+        <f t="shared" si="166"/>
+        <v>-3746.5942922692748</v>
+      </c>
+      <c r="J169">
+        <f t="shared" si="166"/>
+        <v>9772.4290316768947</v>
+      </c>
+    </row>
+    <row r="170" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A170" s="1">
+        <v>44396</v>
+      </c>
+      <c r="B170" t="s">
+        <v>21</v>
+      </c>
+      <c r="C170" t="s">
+        <v>24</v>
+      </c>
+      <c r="D170">
+        <f>D164+D169</f>
+        <v>5000760.789576536</v>
+      </c>
+      <c r="E170">
+        <f t="shared" ref="E170:J170" si="167">E164+E169</f>
+        <v>601630.93205651315</v>
+      </c>
+      <c r="F170">
+        <f t="shared" si="167"/>
+        <v>508448.68397577084</v>
+      </c>
+      <c r="G170">
+        <f t="shared" si="167"/>
+        <v>178358.84310382171</v>
+      </c>
+      <c r="H170">
+        <f t="shared" si="167"/>
+        <v>563189.17213787592</v>
+      </c>
+      <c r="I170">
+        <f t="shared" si="167"/>
+        <v>-3746.5942922692748</v>
+      </c>
+      <c r="J170">
+        <f t="shared" si="167"/>
+        <v>9772.4290316768947</v>
+      </c>
+    </row>
+    <row r="171" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A171" s="1">
+        <v>44396</v>
+      </c>
+      <c r="B171" t="s">
+        <v>21</v>
+      </c>
+      <c r="C171" t="s">
+        <v>25</v>
+      </c>
+      <c r="D171">
+        <f>D170/SUM($D170:$J170)</f>
+        <v>0.72914242319216649</v>
+      </c>
+      <c r="E171">
+        <f t="shared" ref="E171" si="168">E170/SUM($D170:$J170)</f>
+        <v>8.7721579600730029E-2</v>
+      </c>
+      <c r="F171">
+        <f t="shared" ref="F171:J171" si="169">F170/SUM($D170:$J170)</f>
+        <v>7.4135020870365428E-2</v>
+      </c>
+      <c r="G171">
+        <f t="shared" si="169"/>
+        <v>2.6005842816865576E-2</v>
+      </c>
+      <c r="H171">
+        <f t="shared" si="169"/>
+        <v>8.2116528857796939E-2</v>
+      </c>
+      <c r="I171">
+        <f t="shared" si="169"/>
+        <v>-5.4627704781985535E-4</v>
+      </c>
+      <c r="J171">
+        <f t="shared" si="169"/>
+        <v>1.4248817098955365E-3</v>
+      </c>
+    </row>
+    <row r="172" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A172" s="1">
+        <v>44410</v>
+      </c>
+      <c r="B172" t="s">
+        <v>18</v>
+      </c>
+      <c r="C172" t="s">
+        <v>26</v>
+      </c>
+      <c r="D172">
+        <v>0.64</v>
+      </c>
+      <c r="E172">
+        <v>0.52</v>
+      </c>
+      <c r="F172">
+        <v>0.66</v>
+      </c>
+      <c r="G172">
+        <v>0.92</v>
+      </c>
+      <c r="H172">
+        <v>0.3</v>
+      </c>
+      <c r="O172">
+        <v>469225.79599999997</v>
+      </c>
+      <c r="P172">
+        <v>511877.33199999999</v>
+      </c>
+      <c r="Q172">
+        <v>183840</v>
+      </c>
+      <c r="R172">
+        <v>99881.19</v>
+      </c>
+      <c r="S172">
+        <v>31570.628000000001</v>
+      </c>
+    </row>
+    <row r="173" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A173" s="1">
+        <v>44410</v>
+      </c>
+      <c r="B173" t="s">
+        <v>18</v>
+      </c>
+      <c r="C173" t="s">
+        <v>19</v>
+      </c>
+      <c r="D173">
+        <f>D172*O172</f>
+        <v>300304.50943999999</v>
+      </c>
+      <c r="E173">
+        <f>E172*P172</f>
+        <v>266176.21263999998</v>
+      </c>
+      <c r="F173">
+        <f>F172*Q172</f>
+        <v>121334.40000000001</v>
+      </c>
+      <c r="G173">
+        <f>G172*R172</f>
+        <v>91890.694800000012</v>
+      </c>
+      <c r="H173">
+        <f>H172*S172</f>
+        <v>9471.1883999999991</v>
+      </c>
+      <c r="K173">
+        <v>1054674</v>
+      </c>
+      <c r="L173">
+        <f>K173-(SUM(D173:H173))</f>
+        <v>265496.99471999996</v>
+      </c>
+      <c r="O173">
+        <v>469225.79599999997</v>
+      </c>
+      <c r="P173">
+        <v>511877.33199999999</v>
+      </c>
+      <c r="Q173">
+        <v>183840</v>
+      </c>
+      <c r="R173">
+        <v>99881.19</v>
+      </c>
+      <c r="S173">
+        <v>31570.628000000001</v>
+      </c>
+    </row>
+    <row r="174" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A174" s="1">
+        <v>44410</v>
+      </c>
+      <c r="B174" t="s">
+        <v>18</v>
+      </c>
+      <c r="C174" t="s">
+        <v>20</v>
+      </c>
+      <c r="D174">
+        <f>D173+(D173/(SUM($D173:$H173)))*$L173</f>
+        <v>401333.73890785006</v>
+      </c>
+      <c r="E174">
+        <f t="shared" ref="E174:H174" si="170">E173+(E173/(SUM($D173:$H173)))*$L173</f>
+        <v>355723.91112723388</v>
+      </c>
+      <c r="F174">
+        <f t="shared" si="170"/>
+        <v>162154.03658422217</v>
+      </c>
+      <c r="G174">
+        <f t="shared" si="170"/>
+        <v>122804.80297713421</v>
+      </c>
+      <c r="H174">
+        <f t="shared" si="170"/>
+        <v>12657.510403559587</v>
+      </c>
+    </row>
+    <row r="175" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A175" s="1">
+        <v>44410</v>
+      </c>
+      <c r="B175" t="s">
+        <v>21</v>
+      </c>
+      <c r="C175" t="s">
+        <v>28</v>
+      </c>
+      <c r="D175">
+        <v>0.83</v>
+      </c>
+      <c r="E175">
+        <v>0.05</v>
+      </c>
+      <c r="F175">
+        <v>0.06</v>
+      </c>
+      <c r="G175">
+        <v>0.01</v>
+      </c>
+      <c r="H175">
+        <v>0.1</v>
+      </c>
+      <c r="I175" s="5">
+        <v>2.156462782801142E-4</v>
+      </c>
+      <c r="J175" s="4">
+        <v>1.7674898883607312E-3</v>
+      </c>
+    </row>
+    <row r="176" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A176" s="1">
+        <v>44410</v>
+      </c>
+      <c r="B176" t="s">
+        <v>21</v>
+      </c>
+      <c r="C176" t="s">
+        <v>19</v>
+      </c>
+      <c r="D176">
+        <f>D175*$K176</f>
+        <v>4967759.99</v>
+      </c>
+      <c r="E176">
+        <f t="shared" ref="E176:J176" si="171">E175*$K176</f>
+        <v>299262.65000000002</v>
+      </c>
+      <c r="F176">
+        <f t="shared" si="171"/>
+        <v>359115.18</v>
+      </c>
+      <c r="G176">
+        <f t="shared" si="171"/>
+        <v>59852.53</v>
+      </c>
+      <c r="H176">
+        <f t="shared" si="171"/>
+        <v>598525.30000000005</v>
+      </c>
+      <c r="I176">
+        <f t="shared" si="171"/>
+        <v>1290.6975340148883</v>
+      </c>
+      <c r="J176">
+        <f t="shared" si="171"/>
+        <v>10578.874156780732</v>
+      </c>
+      <c r="K176" s="2">
+        <v>5985253</v>
+      </c>
+    </row>
+    <row r="177" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A177" s="1">
+        <v>44410</v>
+      </c>
+      <c r="B177" t="s">
+        <v>21</v>
+      </c>
+      <c r="C177" t="s">
+        <v>29</v>
+      </c>
+      <c r="D177">
+        <v>0.77694459599999999</v>
+      </c>
+      <c r="E177">
+        <v>0.10407799600000001</v>
+      </c>
+      <c r="G177">
+        <v>4.0013660000000001E-3</v>
+      </c>
+      <c r="H177">
+        <v>0.10407799600000001</v>
+      </c>
+      <c r="I177">
+        <v>1.4221746E-2</v>
+      </c>
+      <c r="J177">
+        <v>1.737557E-3</v>
+      </c>
+      <c r="K177" s="2"/>
+    </row>
+    <row r="178" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A178" s="1">
+        <v>44410</v>
+      </c>
+      <c r="B178" t="s">
+        <v>21</v>
+      </c>
+      <c r="C178" t="s">
+        <v>22</v>
+      </c>
+      <c r="D178">
+        <f>$F176*D177</f>
+        <v>279012.59844256728</v>
+      </c>
+      <c r="E178">
+        <f t="shared" ref="E178:J178" si="172">$F176*E177</f>
+        <v>37375.988267579283</v>
+      </c>
+      <c r="F178">
+        <f t="shared" si="172"/>
+        <v>0</v>
+      </c>
+      <c r="G178">
+        <f t="shared" si="172"/>
+        <v>1436.9512713358799</v>
+      </c>
+      <c r="H178">
+        <f t="shared" si="172"/>
+        <v>37375.988267579283</v>
+      </c>
+      <c r="I178">
+        <f t="shared" si="172"/>
+        <v>5107.2448747042799</v>
+      </c>
+      <c r="J178">
+        <f t="shared" si="172"/>
+        <v>623.98309481525996</v>
+      </c>
+    </row>
+    <row r="179" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A179" s="1">
+        <v>44410</v>
+      </c>
+      <c r="B179" t="s">
+        <v>21</v>
+      </c>
+      <c r="C179" t="s">
+        <v>23</v>
+      </c>
+      <c r="D179">
+        <f>D176-D178</f>
+        <v>4688747.3915574327</v>
+      </c>
+      <c r="E179">
+        <f t="shared" ref="E179:J179" si="173">E176-E178</f>
+        <v>261886.66173242073</v>
+      </c>
+      <c r="F179">
+        <f t="shared" si="173"/>
+        <v>359115.18</v>
+      </c>
+      <c r="G179">
+        <f t="shared" si="173"/>
+        <v>58415.578728664121</v>
+      </c>
+      <c r="H179">
+        <f t="shared" si="173"/>
+        <v>561149.31173242081</v>
+      </c>
+      <c r="I179">
+        <f t="shared" si="173"/>
+        <v>-3816.5473406893916</v>
+      </c>
+      <c r="J179">
+        <f t="shared" si="173"/>
+        <v>9954.8910619654725</v>
+      </c>
+    </row>
+    <row r="180" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A180" s="1">
+        <v>44410</v>
+      </c>
+      <c r="B180" t="s">
+        <v>21</v>
+      </c>
+      <c r="C180" t="s">
+        <v>24</v>
+      </c>
+      <c r="D180">
+        <f>D174+D179</f>
+        <v>5090081.1304652831</v>
+      </c>
+      <c r="E180">
+        <f t="shared" ref="E180:J180" si="174">E174+E179</f>
+        <v>617610.57285965467</v>
+      </c>
+      <c r="F180">
+        <f t="shared" si="174"/>
+        <v>521269.21658422216</v>
+      </c>
+      <c r="G180">
+        <f t="shared" si="174"/>
+        <v>181220.38170579833</v>
+      </c>
+      <c r="H180">
+        <f t="shared" si="174"/>
+        <v>573806.82213598036</v>
+      </c>
+      <c r="I180">
+        <f t="shared" si="174"/>
+        <v>-3816.5473406893916</v>
+      </c>
+      <c r="J180">
+        <f t="shared" si="174"/>
+        <v>9954.8910619654725</v>
+      </c>
+    </row>
+    <row r="181" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A181" s="1">
+        <v>44410</v>
+      </c>
+      <c r="B181" t="s">
+        <v>21</v>
+      </c>
+      <c r="C181" t="s">
+        <v>25</v>
+      </c>
+      <c r="D181">
+        <f>D180/SUM($D180:$J180)</f>
+        <v>0.72818155067027979</v>
+      </c>
+      <c r="E181">
+        <f t="shared" ref="E181" si="175">E180/SUM($D180:$J180)</f>
+        <v>8.8354706561267177E-2</v>
+      </c>
+      <c r="F181">
+        <f t="shared" ref="F181:J181" si="176">F180/SUM($D180:$J180)</f>
+        <v>7.4572215396944697E-2</v>
+      </c>
+      <c r="G181">
+        <f t="shared" si="176"/>
+        <v>2.5925193563963032E-2</v>
+      </c>
+      <c r="H181">
+        <f t="shared" si="176"/>
+        <v>8.208818893422419E-2</v>
+      </c>
+      <c r="I181">
+        <f t="shared" si="176"/>
+        <v>-5.4599117175479941E-4</v>
+      </c>
+      <c r="J181">
+        <f t="shared" si="176"/>
+        <v>1.4241360450757885E-3</v>
+      </c>
+    </row>
+    <row r="182" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A182" s="1">
+        <v>44424</v>
+      </c>
+      <c r="B182" t="s">
+        <v>18</v>
+      </c>
+      <c r="C182" t="s">
+        <v>26</v>
+      </c>
+      <c r="D182">
+        <v>0.65</v>
+      </c>
+      <c r="E182">
+        <v>0.53</v>
+      </c>
+      <c r="F182">
+        <v>0.69</v>
+      </c>
+      <c r="G182">
+        <v>0.93</v>
+      </c>
+      <c r="H182">
+        <v>0.31</v>
+      </c>
+      <c r="O182">
+        <v>469225.79599999997</v>
+      </c>
+      <c r="P182">
+        <v>511877.33199999999</v>
+      </c>
+      <c r="Q182">
+        <v>183840</v>
+      </c>
+      <c r="R182">
+        <v>99881.19</v>
+      </c>
+      <c r="S182">
+        <v>31570.628000000001</v>
+      </c>
+    </row>
+    <row r="183" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A183" s="1">
+        <v>44424</v>
+      </c>
+      <c r="B183" t="s">
+        <v>18</v>
+      </c>
+      <c r="C183" t="s">
+        <v>19</v>
+      </c>
+      <c r="D183">
+        <f>D182*O182</f>
+        <v>304996.76740000001</v>
+      </c>
+      <c r="E183">
+        <f>E182*P182</f>
+        <v>271294.98596000002</v>
+      </c>
+      <c r="F183">
+        <f>F182*Q182</f>
+        <v>126849.59999999999</v>
+      </c>
+      <c r="G183">
+        <f>G182*R182</f>
+        <v>92889.506700000013</v>
+      </c>
+      <c r="H183">
+        <f>H182*S182</f>
+        <v>9786.8946799999994</v>
+      </c>
+      <c r="K183">
+        <v>1079387</v>
+      </c>
+      <c r="L183">
+        <f>K183-(SUM(D183:H183))</f>
+        <v>273569.24526</v>
+      </c>
+      <c r="O183">
+        <v>469225.79599999997</v>
+      </c>
+      <c r="P183">
+        <v>511877.33199999999</v>
+      </c>
+      <c r="Q183">
+        <v>183840</v>
+      </c>
+      <c r="R183">
+        <v>99881.19</v>
+      </c>
+      <c r="S183">
+        <v>31570.628000000001</v>
+      </c>
+    </row>
+    <row r="184" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A184" s="1">
+        <v>44424</v>
+      </c>
+      <c r="B184" t="s">
+        <v>18</v>
+      </c>
+      <c r="C184" t="s">
+        <v>20</v>
+      </c>
+      <c r="D184">
+        <f>D183+(D183/(SUM($D183:$H183)))*$L183</f>
+        <v>408540.94345414918</v>
+      </c>
+      <c r="E184">
+        <f t="shared" ref="E184:H184" si="177">E183+(E183/(SUM($D183:$H183)))*$L183</f>
+        <v>363397.65323846694</v>
+      </c>
+      <c r="F184">
+        <f t="shared" si="177"/>
+        <v>169914.11319719267</v>
+      </c>
+      <c r="G184">
+        <f t="shared" si="177"/>
+        <v>124424.81613071849</v>
+      </c>
+      <c r="H184">
+        <f t="shared" si="177"/>
+        <v>13109.473979472719</v>
+      </c>
+    </row>
+    <row r="185" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A185" s="1">
+        <v>44424</v>
+      </c>
+      <c r="B185" t="s">
+        <v>21</v>
+      </c>
+      <c r="C185" t="s">
+        <v>28</v>
+      </c>
+      <c r="D185">
+        <v>0.8</v>
+      </c>
+      <c r="E185">
+        <v>0.06</v>
+      </c>
+      <c r="F185">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="G185">
+        <v>0.01</v>
+      </c>
+      <c r="H185">
+        <v>0.12</v>
+      </c>
+      <c r="I185" s="5">
+        <v>2.156462782801142E-4</v>
+      </c>
+      <c r="J185" s="4">
+        <v>1.7674898883607312E-3</v>
+      </c>
+    </row>
+    <row r="186" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A186" s="1">
+        <v>44424</v>
+      </c>
+      <c r="B186" t="s">
+        <v>21</v>
+      </c>
+      <c r="C186" t="s">
+        <v>19</v>
+      </c>
+      <c r="D186">
+        <f>D185*$K186</f>
+        <v>4888502.4000000004</v>
+      </c>
+      <c r="E186">
+        <f t="shared" ref="E186:J186" si="178">E185*$K186</f>
+        <v>366637.68</v>
+      </c>
+      <c r="F186">
+        <f t="shared" si="178"/>
+        <v>427743.96</v>
+      </c>
+      <c r="G186">
+        <f t="shared" si="178"/>
+        <v>61106.28</v>
+      </c>
+      <c r="H186">
+        <f t="shared" si="178"/>
+        <v>733275.36</v>
+      </c>
+      <c r="I186">
+        <f t="shared" si="178"/>
+        <v>1317.7341861542577</v>
+      </c>
+      <c r="J186">
+        <f t="shared" si="178"/>
+        <v>10800.473201533958</v>
+      </c>
+      <c r="K186" s="2">
+        <v>6110628</v>
+      </c>
+    </row>
+    <row r="187" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A187" s="1">
+        <v>44424</v>
+      </c>
+      <c r="B187" t="s">
+        <v>21</v>
+      </c>
+      <c r="C187" t="s">
+        <v>29</v>
+      </c>
+      <c r="D187">
+        <v>0.77694459599999999</v>
+      </c>
+      <c r="E187">
+        <v>0.10407799600000001</v>
+      </c>
+      <c r="G187">
+        <v>4.0013660000000001E-3</v>
+      </c>
+      <c r="H187">
+        <v>0.10407799600000001</v>
+      </c>
+      <c r="I187">
+        <v>1.4221746E-2</v>
+      </c>
+      <c r="J187">
+        <v>1.737557E-3</v>
+      </c>
+      <c r="K187" s="2"/>
+    </row>
+    <row r="188" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A188" s="1">
+        <v>44424</v>
+      </c>
+      <c r="B188" t="s">
+        <v>21</v>
+      </c>
+      <c r="C188" t="s">
+        <v>22</v>
+      </c>
+      <c r="D188">
+        <f>$F186*D187</f>
+        <v>332333.35819364019</v>
+      </c>
+      <c r="E188">
+        <f t="shared" ref="E188:J188" si="179">$F186*E187</f>
+        <v>44518.734157904168</v>
+      </c>
+      <c r="F188">
+        <f t="shared" si="179"/>
+        <v>0</v>
+      </c>
+      <c r="G188">
+        <f t="shared" si="179"/>
+        <v>1711.5601382493601</v>
+      </c>
+      <c r="H188">
+        <f t="shared" si="179"/>
+        <v>44518.734157904168</v>
+      </c>
+      <c r="I188">
+        <f t="shared" si="179"/>
+        <v>6083.2659521541609</v>
+      </c>
+      <c r="J188">
+        <f t="shared" si="179"/>
+        <v>743.22951190572007</v>
+      </c>
+    </row>
+    <row r="189" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A189" s="1">
+        <v>44424</v>
+      </c>
+      <c r="B189" t="s">
+        <v>21</v>
+      </c>
+      <c r="C189" t="s">
+        <v>23</v>
+      </c>
+      <c r="D189">
+        <f>D186-D188</f>
+        <v>4556169.0418063598</v>
+      </c>
+      <c r="E189">
+        <f t="shared" ref="E189:J189" si="180">E186-E188</f>
+        <v>322118.94584209583</v>
+      </c>
+      <c r="F189">
+        <f t="shared" si="180"/>
+        <v>427743.96</v>
+      </c>
+      <c r="G189">
+        <f t="shared" si="180"/>
+        <v>59394.719861750636</v>
+      </c>
+      <c r="H189">
+        <f t="shared" si="180"/>
+        <v>688756.62584209582</v>
+      </c>
+      <c r="I189">
+        <f t="shared" si="180"/>
+        <v>-4765.5317659999037</v>
+      </c>
+      <c r="J189">
+        <f t="shared" si="180"/>
+        <v>10057.243689628238</v>
+      </c>
+    </row>
+    <row r="190" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A190" s="1">
+        <v>44424</v>
+      </c>
+      <c r="B190" t="s">
+        <v>21</v>
+      </c>
+      <c r="C190" t="s">
+        <v>24</v>
+      </c>
+      <c r="D190">
+        <f>D184+D189</f>
+        <v>4964709.985260509</v>
+      </c>
+      <c r="E190">
+        <f t="shared" ref="E190:J190" si="181">E184+E189</f>
+        <v>685516.59908056282</v>
+      </c>
+      <c r="F190">
+        <f t="shared" si="181"/>
+        <v>597658.07319719275</v>
+      </c>
+      <c r="G190">
+        <f t="shared" si="181"/>
+        <v>183819.53599246911</v>
+      </c>
+      <c r="H190">
+        <f t="shared" si="181"/>
+        <v>701866.09982156858</v>
+      </c>
+      <c r="I190">
+        <f t="shared" si="181"/>
+        <v>-4765.5317659999037</v>
+      </c>
+      <c r="J190">
+        <f t="shared" si="181"/>
+        <v>10057.243689628238</v>
+      </c>
+    </row>
+    <row r="191" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A191" s="1">
+        <v>44424</v>
+      </c>
+      <c r="B191" t="s">
+        <v>21</v>
+      </c>
+      <c r="C191" t="s">
+        <v>25</v>
+      </c>
+      <c r="D191">
+        <f>D190/SUM($D190:$J190)</f>
+        <v>0.69544837560823736</v>
+      </c>
+      <c r="E191">
+        <f t="shared" ref="E191" si="182">E190/SUM($D190:$J190)</f>
+        <v>9.6026033081174036E-2</v>
+      </c>
+      <c r="F191">
+        <f t="shared" ref="F191:J191" si="183">F190/SUM($D190:$J190)</f>
+        <v>8.3718955872168058E-2</v>
+      </c>
+      <c r="G191">
+        <f t="shared" si="183"/>
+        <v>2.574913702724867E-2</v>
+      </c>
+      <c r="H191">
+        <f t="shared" si="183"/>
+        <v>9.831624414407493E-2</v>
+      </c>
+      <c r="I191">
+        <f t="shared" si="183"/>
+        <v>-6.675478195933706E-4</v>
+      </c>
+      <c r="J191">
+        <f t="shared" si="183"/>
+        <v>1.4088020866904975E-3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>